<commit_message>
fix live-edit and live-delete
</commit_message>
<xml_diff>
--- a/Data for tests/test1.XLSX
+++ b/Data for tests/test1.XLSX
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programming\projects\JavaProgramming\ShrekWebApp\Data for tests\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programming\ShrekWebApp\Data for tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{547AFA42-0E9A-488D-8C5D-0BAEB95E6C6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F3ABBB7-60BF-43A7-BA07-8B0D62AE927F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
     <t>00ppss88@test.rf</t>
   </si>
   <si>
-    <t>Name</t>
+    <t>Name + авава* dfd</t>
   </si>
 </sst>
 </file>
@@ -374,7 +374,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>